<commit_message>
Working but errors in multiple undos
</commit_message>
<xml_diff>
--- a/BOBanker/data archives/BOAnalytics20.xlsx
+++ b/BOBanker/data archives/BOAnalytics20.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\BO\BOBanker\BOBanker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Desktop\BO\BOBanker\BOBanker\data archives\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7620" firstSheet="3" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="PlayerNetWorth" sheetId="2" r:id="rId1"/>
@@ -20314,7 +20314,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21063,7 +21062,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -21140,7 +21138,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22482,7 +22479,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -22559,7 +22555,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23898,7 +23893,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -23975,7 +23969,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25315,7 +25308,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25392,7 +25384,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -26754,7 +26745,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -31833,8 +31823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BM237"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="BC187" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D216" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="A189" sqref="A189:XFD189"/>
@@ -78767,13 +78757,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CQ26"/>
+  <dimension ref="A1:CQ27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="BX22" sqref="BX22"/>
+      <selection pane="bottomRight" activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -79319,43 +79309,43 @@
         <v>0</v>
       </c>
       <c r="CH2" s="1">
-        <f>BX2/AI2</f>
+        <f t="shared" ref="CH2:CH26" si="0">BX2/AI2</f>
         <v>0</v>
       </c>
       <c r="CI2" s="1">
-        <f>BY2/AJ2</f>
+        <f t="shared" ref="CI2:CI26" si="1">BY2/AJ2</f>
         <v>0</v>
       </c>
       <c r="CJ2" s="1">
-        <f>BZ2/AK2</f>
+        <f t="shared" ref="CJ2:CJ26" si="2">BZ2/AK2</f>
         <v>0</v>
       </c>
       <c r="CK2" s="1">
-        <f>CA2/AL2</f>
+        <f t="shared" ref="CK2:CK26" si="3">CA2/AL2</f>
         <v>0</v>
       </c>
       <c r="CL2" s="1">
-        <f>CB2/AM2</f>
+        <f t="shared" ref="CL2:CL26" si="4">CB2/AM2</f>
         <v>0</v>
       </c>
       <c r="CM2" s="1">
-        <f>CC2/AN2</f>
+        <f t="shared" ref="CM2:CM26" si="5">CC2/AN2</f>
         <v>0</v>
       </c>
       <c r="CN2" s="1">
-        <f>CD2/AO2</f>
+        <f t="shared" ref="CN2:CN26" si="6">CD2/AO2</f>
         <v>0</v>
       </c>
       <c r="CO2" s="1">
-        <f>CE2/AP2</f>
+        <f t="shared" ref="CO2:CO26" si="7">CE2/AP2</f>
         <v>0</v>
       </c>
       <c r="CP2" s="1">
-        <f>CF2/AQ2</f>
+        <f t="shared" ref="CP2:CP26" si="8">CF2/AQ2</f>
         <v>0</v>
       </c>
       <c r="CQ2" s="1">
-        <f>CG2/AR2</f>
+        <f t="shared" ref="CQ2:CQ26" si="9">CG2/AR2</f>
         <v>0</v>
       </c>
     </row>
@@ -79623,43 +79613,43 @@
         <v>0</v>
       </c>
       <c r="CH3" s="1">
-        <f>BX3/AI3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="CI3" s="1">
-        <f>BY3/AJ3</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ3" s="1">
-        <f>BZ3/AK3</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK3" s="1">
-        <f>CA3/AL3</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL3" s="1">
-        <f>CB3/AM3</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM3" s="1">
-        <f>CC3/AN3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CN3" s="1">
-        <f>CD3/AO3</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO3" s="1">
-        <f>CE3/AP3</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP3" s="1">
-        <f>CF3/AQ3</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="CQ3" s="1">
-        <f>CG3/AR3</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -79893,77 +79883,77 @@
         <v>0</v>
       </c>
       <c r="BY4">
-        <f>Z4/10*BO4+(AJ4-AJ3)</f>
+        <f t="shared" ref="BY4:CB11" si="10">Z4/10*BO4+(AJ4-AJ3)</f>
         <v>0</v>
       </c>
       <c r="BZ4">
-        <f>AA4/10*BP4+(AK4-AK3)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CA4">
-        <f>AB4/10*BQ4+(AL4-AL3)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CB4">
-        <f>AC4/10*BR4+(AM4-AM3)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CC4">
         <v>0</v>
       </c>
       <c r="CD4">
-        <f>AE4/10*BT4+(AO4-AO3)</f>
+        <f t="shared" ref="CD4:CD17" si="11">AE4/10*BT4+(AO4-AO3)</f>
         <v>0</v>
       </c>
       <c r="CE4">
-        <f>AF4/10*BU4+(AP4-AP3)</f>
+        <f t="shared" ref="CE4:CE17" si="12">AF4/10*BU4+(AP4-AP3)</f>
         <v>0</v>
       </c>
       <c r="CF4">
         <v>0</v>
       </c>
       <c r="CG4">
-        <f>AH4/10*BW4+(AR4-AR3)</f>
+        <f t="shared" ref="CG4:CG20" si="13">AH4/10*BW4+(AR4-AR3)</f>
         <v>0</v>
       </c>
       <c r="CH4" s="1">
-        <f>BX4/AI4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="CI4" s="1">
-        <f>BY4/AJ4</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ4" s="1">
-        <f>BZ4/AK4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK4" s="1">
-        <f>CA4/AL4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL4" s="1">
-        <f>CB4/AM4</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM4" s="1">
-        <f>CC4/AN4</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CN4" s="1">
-        <f>CD4/AO4</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO4" s="1">
-        <f>CE4/AP4</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP4" s="1">
-        <f>CF4/AQ4</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="CQ4" s="1">
-        <f>CG4/AR4</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -80194,83 +80184,83 @@
         <v>1</v>
       </c>
       <c r="BX5">
-        <f>Y5/10*BN5+(AI5-AI4)</f>
+        <f t="shared" ref="BX5:BX26" si="14">Y5/10*BN5+(AI5-AI4)</f>
         <v>1</v>
       </c>
       <c r="BY5">
-        <f>Z5/10*BO5+(AJ5-AJ4)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BZ5">
-        <f>AA5/10*BP5+(AK5-AK4)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CA5">
-        <f>AB5/10*BQ5+(AL5-AL4)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CB5">
-        <f>AC5/10*BR5+(AM5-AM4)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CC5">
-        <f>AD5/10*BS5+(AN5-AN4)</f>
+        <f t="shared" ref="CC5:CC26" si="15">AD5/10*BS5+(AN5-AN4)</f>
         <v>10</v>
       </c>
       <c r="CD5">
-        <f>AE5/10*BT5+(AO5-AO4)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE5">
-        <f>AF5/10*BU5+(AP5-AP4)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF5">
-        <f>AG5/10*BV5+(AQ5-AQ4)</f>
+        <f t="shared" ref="CF5:CF26" si="16">AG5/10*BV5+(AQ5-AQ4)</f>
         <v>2</v>
       </c>
       <c r="CG5">
-        <f>AH5/10*BW5+(AR5-AR4)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH5" s="1">
-        <f>BX5/AI5</f>
+        <f t="shared" si="0"/>
         <v>1.3513513513513514E-2</v>
       </c>
       <c r="CI5" s="1">
-        <f>BY5/AJ5</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ5" s="1">
-        <f>BZ5/AK5</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK5" s="1">
-        <f>CA5/AL5</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL5" s="1">
-        <f>CB5/AM5</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM5" s="1">
-        <f>CC5/AN5</f>
+        <f t="shared" si="5"/>
         <v>0.15151515151515152</v>
       </c>
       <c r="CN5" s="1">
-        <f>CD5/AO5</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO5" s="1">
-        <f>CE5/AP5</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP5" s="1">
-        <f>CF5/AQ5</f>
+        <f t="shared" si="8"/>
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="CQ5" s="1">
-        <f>CG5/AR5</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -80501,83 +80491,83 @@
         <v>0</v>
       </c>
       <c r="BX6">
-        <f>Y6/10*BN6+(AI6-AI5)</f>
+        <f t="shared" si="14"/>
         <v>-8</v>
       </c>
       <c r="BY6">
-        <f>Z6/10*BO6+(AJ6-AJ5)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BZ6">
-        <f>AA6/10*BP6+(AK6-AK5)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CA6">
-        <f>AB6/10*BQ6+(AL6-AL5)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CB6">
-        <f>AC6/10*BR6+(AM6-AM5)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CC6">
-        <f>AD6/10*BS6+(AN6-AN5)</f>
+        <f t="shared" si="15"/>
         <v>-6</v>
       </c>
       <c r="CD6">
-        <f>AE6/10*BT6+(AO6-AO5)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE6">
-        <f>AF6/10*BU6+(AP6-AP5)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF6">
-        <f>AG6/10*BV6+(AQ6-AQ5)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="CG6">
-        <f>AH6/10*BW6+(AR6-AR5)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH6" s="1">
-        <f>BX6/AI6</f>
+        <f t="shared" si="0"/>
         <v>-0.12121212121212122</v>
       </c>
       <c r="CI6" s="1">
-        <f>BY6/AJ6</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ6" s="1">
-        <f>BZ6/AK6</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK6" s="1">
-        <f>CA6/AL6</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL6" s="1">
-        <f>CB6/AM6</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM6" s="1">
-        <f>CC6/AN6</f>
+        <f t="shared" si="5"/>
         <v>-0.1</v>
       </c>
       <c r="CN6" s="1">
-        <f>CD6/AO6</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO6" s="1">
-        <f>CE6/AP6</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP6" s="1">
-        <f>CF6/AQ6</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="CQ6" s="1">
-        <f>CG6/AR6</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -80808,83 +80798,83 @@
         <v>1</v>
       </c>
       <c r="BX7">
-        <f>Y7/10*BN7+(AI7-AI6)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="BY7">
-        <f>Z7/10*BO7+(AJ7-AJ6)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BZ7">
-        <f>AA7/10*BP7+(AK7-AK6)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CA7">
-        <f>AB7/10*BQ7+(AL7-AL6)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CB7">
-        <f>AC7/10*BR7+(AM7-AM6)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CC7">
-        <f>AD7/10*BS7+(AN7-AN6)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="CD7">
-        <f>AE7/10*BT7+(AO7-AO6)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE7">
-        <f>AF7/10*BU7+(AP7-AP6)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF7">
-        <f>AG7/10*BV7+(AQ7-AQ6)</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="CG7">
-        <f>AH7/10*BW7+(AR7-AR6)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH7" s="1">
-        <f>BX7/AI7</f>
+        <f t="shared" si="0"/>
         <v>1.5151515151515152E-2</v>
       </c>
       <c r="CI7" s="1">
-        <f>BY7/AJ7</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ7" s="1">
-        <f>BZ7/AK7</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK7" s="1">
-        <f>CA7/AL7</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL7" s="1">
-        <f>CB7/AM7</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM7" s="1">
-        <f>CC7/AN7</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CN7" s="1">
-        <f>CD7/AO7</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO7" s="1">
-        <f>CE7/AP7</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP7" s="1">
-        <f>CF7/AQ7</f>
+        <f t="shared" si="8"/>
         <v>3.0303030303030304E-2</v>
       </c>
       <c r="CQ7" s="1">
-        <f>CG7/AR7</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -81115,83 +81105,83 @@
         <v>1</v>
       </c>
       <c r="BX8">
-        <f>Y8/10*BN8+(AI8-AI7)</f>
+        <f t="shared" si="14"/>
         <v>13</v>
       </c>
       <c r="BY8">
-        <f>Z8/10*BO8+(AJ8-AJ7)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BZ8">
-        <f>AA8/10*BP8+(AK8-AK7)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CA8">
-        <f>AB8/10*BQ8+(AL8-AL7)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CB8">
-        <f>AC8/10*BR8+(AM8-AM7)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CC8">
-        <f>AD8/10*BS8+(AN8-AN7)</f>
+        <f t="shared" si="15"/>
         <v>4</v>
       </c>
       <c r="CD8">
-        <f>AE8/10*BT8+(AO8-AO7)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE8">
-        <f>AF8/10*BU8+(AP8-AP7)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF8">
-        <f>AG8/10*BV8+(AQ8-AQ7)</f>
+        <f t="shared" si="16"/>
         <v>14</v>
       </c>
       <c r="CG8">
-        <f>AH8/10*BW8+(AR8-AR7)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH8" s="1">
-        <f>BX8/AI8</f>
+        <f t="shared" si="0"/>
         <v>0.17567567567567569</v>
       </c>
       <c r="CI8" s="1">
-        <f>BY8/AJ8</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ8" s="1">
-        <f>BZ8/AK8</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK8" s="1">
-        <f>CA8/AL8</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL8" s="1">
-        <f>CB8/AM8</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM8" s="1">
-        <f>CC8/AN8</f>
+        <f t="shared" si="5"/>
         <v>6.6666666666666666E-2</v>
       </c>
       <c r="CN8" s="1">
-        <f>CD8/AO8</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO8" s="1">
-        <f>CE8/AP8</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP8" s="1">
-        <f>CF8/AQ8</f>
+        <f t="shared" si="8"/>
         <v>0.1891891891891892</v>
       </c>
       <c r="CQ8" s="1">
-        <f>CG8/AR8</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -81422,83 +81412,83 @@
         <v>0</v>
       </c>
       <c r="BX9">
-        <f>Y9/10*BN9+(AI9-AI8)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BY9">
-        <f>Z9/10*BO9+(AJ9-AJ8)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BZ9">
-        <f>AA9/10*BP9+(AK9-AK8)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CA9">
-        <f>AB9/10*BQ9+(AL9-AL8)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CB9">
-        <f>AC9/10*BR9+(AM9-AM8)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CC9">
-        <f>AD9/10*BS9+(AN9-AN8)</f>
+        <f t="shared" si="15"/>
         <v>-5</v>
       </c>
       <c r="CD9">
-        <f>AE9/10*BT9+(AO9-AO8)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE9">
-        <f>AF9/10*BU9+(AP9-AP8)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF9">
-        <f>AG9/10*BV9+(AQ9-AQ8)</f>
+        <f t="shared" si="16"/>
         <v>-8</v>
       </c>
       <c r="CG9">
-        <f>AH9/10*BW9+(AR9-AR8)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH9" s="1">
-        <f>BX9/AI9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="CI9" s="1">
-        <f>BY9/AJ9</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ9" s="1">
-        <f>BZ9/AK9</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK9" s="1">
-        <f>CA9/AL9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL9" s="1">
-        <f>CB9/AM9</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM9" s="1">
-        <f>CC9/AN9</f>
+        <f t="shared" si="5"/>
         <v>-9.0909090909090912E-2</v>
       </c>
       <c r="CN9" s="1">
-        <f>CD9/AO9</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO9" s="1">
-        <f>CE9/AP9</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP9" s="1">
-        <f>CF9/AQ9</f>
+        <f t="shared" si="8"/>
         <v>-0.12121212121212122</v>
       </c>
       <c r="CQ9" s="1">
-        <f>CG9/AR9</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -81729,83 +81719,83 @@
         <v>1</v>
       </c>
       <c r="BX10">
-        <f>Y10/10*BN10+(AI10-AI9)</f>
+        <f t="shared" si="14"/>
         <v>14</v>
       </c>
       <c r="BY10">
-        <f>Z10/10*BO10+(AJ10-AJ9)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BZ10">
-        <f>AA10/10*BP10+(AK10-AK9)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CA10">
-        <f>AB10/10*BQ10+(AL10-AL9)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CB10">
-        <f>AC10/10*BR10+(AM10-AM9)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CC10">
-        <f>AD10/10*BS10+(AN10-AN9)</f>
+        <f t="shared" si="15"/>
         <v>10</v>
       </c>
       <c r="CD10">
-        <f>AE10/10*BT10+(AO10-AO9)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE10">
-        <f>AF10/10*BU10+(AP10-AP9)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF10">
-        <f>AG10/10*BV10+(AQ10-AQ9)</f>
+        <f t="shared" si="16"/>
         <v>17</v>
       </c>
       <c r="CG10">
-        <f>AH10/10*BW10+(AR10-AR9)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH10" s="1">
-        <f>BX10/AI10</f>
+        <f t="shared" si="0"/>
         <v>0.17073170731707318</v>
       </c>
       <c r="CI10" s="1">
-        <f>BY10/AJ10</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ10" s="1">
-        <f>BZ10/AK10</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK10" s="1">
-        <f>CA10/AL10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL10" s="1">
-        <f>CB10/AM10</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM10" s="1">
-        <f>CC10/AN10</f>
+        <f t="shared" si="5"/>
         <v>0.16666666666666666</v>
       </c>
       <c r="CN10" s="1">
-        <f>CD10/AO10</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO10" s="1">
-        <f>CE10/AP10</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP10" s="1">
-        <f>CF10/AQ10</f>
+        <f t="shared" si="8"/>
         <v>0.22972972972972974</v>
       </c>
       <c r="CQ10" s="1">
-        <f>CG10/AR10</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -82036,83 +82026,83 @@
         <v>1</v>
       </c>
       <c r="BX11">
-        <f>Y11/10*BN11+(AI11-AI10)</f>
+        <f t="shared" si="14"/>
         <v>18</v>
       </c>
       <c r="BY11">
-        <f>Z11/10*BO11+(AJ11-AJ10)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="BZ11">
-        <f>AA11/10*BP11+(AK11-AK10)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CA11">
-        <f>AB11/10*BQ11+(AL11-AL10)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CB11">
-        <f>AC11/10*BR11+(AM11-AM10)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="CC11">
-        <f>AD11/10*BS11+(AN11-AN10)</f>
+        <f t="shared" si="15"/>
         <v>12</v>
       </c>
       <c r="CD11">
-        <f>AE11/10*BT11+(AO11-AO10)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE11">
-        <f>AF11/10*BU11+(AP11-AP10)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF11">
-        <f>AG11/10*BV11+(AQ11-AQ10)</f>
+        <f t="shared" si="16"/>
         <v>18</v>
       </c>
       <c r="CG11">
-        <f>AH11/10*BW11+(AR11-AR10)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH11" s="1">
-        <f>BX11/AI11</f>
+        <f t="shared" si="0"/>
         <v>0.19780219780219779</v>
       </c>
       <c r="CI11" s="1">
-        <f>BY11/AJ11</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ11" s="1">
-        <f>BZ11/AK11</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK11" s="1">
-        <f>CA11/AL11</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL11" s="1">
-        <f>CB11/AM11</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM11" s="1">
-        <f>CC11/AN11</f>
+        <f t="shared" si="5"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="CN11" s="1">
-        <f>CD11/AO11</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO11" s="1">
-        <f>CE11/AP11</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP11" s="1">
-        <f>CF11/AQ11</f>
+        <f t="shared" si="8"/>
         <v>0.21951219512195122</v>
       </c>
       <c r="CQ11" s="1">
-        <f>CG11/AR11</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -82343,82 +82333,82 @@
         <v>0</v>
       </c>
       <c r="BX12">
-        <f>Y12/10*BN12+(AI12-AI11)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BY12">
         <v>0</v>
       </c>
       <c r="BZ12">
-        <f>AA12/10*BP12+(AK12-AK11)</f>
+        <f t="shared" ref="BZ12:CB14" si="17">AA12/10*BP12+(AK12-AK11)</f>
         <v>0</v>
       </c>
       <c r="CA12">
-        <f>AB12/10*BQ12+(AL12-AL11)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="CB12">
-        <f>AC12/10*BR12+(AM12-AM11)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="CC12">
-        <f>AD12/10*BS12+(AN12-AN11)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="CD12">
-        <f>AE12/10*BT12+(AO12-AO11)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE12">
-        <f>AF12/10*BU12+(AP12-AP11)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF12">
-        <f>AG12/10*BV12+(AQ12-AQ11)</f>
+        <f t="shared" si="16"/>
         <v>-8</v>
       </c>
       <c r="CG12">
-        <f>AH12/10*BW12+(AR12-AR11)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH12" s="1">
-        <f>BX12/AI12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="CI12" s="1">
-        <f>BY12/AJ12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ12" s="1">
-        <f>BZ12/AK12</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK12" s="1">
-        <f>CA12/AL12</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL12" s="1">
-        <f>CB12/AM12</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM12" s="1">
-        <f>CC12/AN12</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CN12" s="1">
-        <f>CD12/AO12</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO12" s="1">
-        <f>CE12/AP12</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP12" s="1">
-        <f>CF12/AQ12</f>
+        <f t="shared" si="8"/>
         <v>-0.10810810810810811</v>
       </c>
       <c r="CQ12" s="1">
-        <f>CG12/AR12</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -82649,83 +82639,83 @@
         <v>1</v>
       </c>
       <c r="BX13">
-        <f>Y13/10*BN13+(AI13-AI12)</f>
+        <f t="shared" si="14"/>
         <v>19</v>
       </c>
       <c r="BY13">
-        <f>Z13/10*BO13+(AJ13-AJ12)</f>
+        <f t="shared" ref="BY13:BY26" si="18">Z13/10*BO13+(AJ13-AJ12)</f>
         <v>9</v>
       </c>
       <c r="BZ13">
-        <f>AA13/10*BP13+(AK13-AK12)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="CA13">
-        <f>AB13/10*BQ13+(AL13-AL12)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="CB13">
-        <f>AC13/10*BR13+(AM13-AM12)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="CC13">
-        <f>AD13/10*BS13+(AN13-AN12)</f>
+        <f t="shared" si="15"/>
         <v>15</v>
       </c>
       <c r="CD13">
-        <f>AE13/10*BT13+(AO13-AO12)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE13">
-        <f>AF13/10*BU13+(AP13-AP12)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF13">
-        <f>AG13/10*BV13+(AQ13-AQ12)</f>
+        <f t="shared" si="16"/>
         <v>11</v>
       </c>
       <c r="CG13">
-        <f>AH13/10*BW13+(AR13-AR12)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH13" s="1">
-        <f>BX13/AI13</f>
+        <f t="shared" si="0"/>
         <v>0.19</v>
       </c>
       <c r="CI13" s="1">
-        <f>BY13/AJ13</f>
+        <f t="shared" si="1"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="CJ13" s="1">
-        <f>BZ13/AK13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK13" s="1">
-        <f>CA13/AL13</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL13" s="1">
-        <f>CB13/AM13</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM13" s="1">
-        <f>CC13/AN13</f>
+        <f t="shared" si="5"/>
         <v>0.20270270270270271</v>
       </c>
       <c r="CN13" s="1">
-        <f>CD13/AO13</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO13" s="1">
-        <f>CE13/AP13</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP13" s="1">
-        <f>CF13/AQ13</f>
+        <f t="shared" si="8"/>
         <v>0.14864864864864866</v>
       </c>
       <c r="CQ13" s="1">
-        <f>CG13/AR13</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -82956,83 +82946,83 @@
         <v>1</v>
       </c>
       <c r="BX14">
-        <f>Y14/10*BN14+(AI14-AI13)</f>
+        <f t="shared" si="14"/>
         <v>24</v>
       </c>
       <c r="BY14">
-        <f>Z14/10*BO14+(AJ14-AJ13)</f>
+        <f t="shared" si="18"/>
         <v>18</v>
       </c>
       <c r="BZ14">
-        <f>AA14/10*BP14+(AK14-AK13)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="CA14">
-        <f>AB14/10*BQ14+(AL14-AL13)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="CB14">
-        <f>AC14/10*BR14+(AM14-AM13)</f>
+        <f t="shared" si="17"/>
         <v>0</v>
       </c>
       <c r="CC14">
-        <f>AD14/10*BS14+(AN14-AN13)</f>
+        <f t="shared" si="15"/>
         <v>18</v>
       </c>
       <c r="CD14">
-        <f>AE14/10*BT14+(AO14-AO13)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE14">
-        <f>AF14/10*BU14+(AP14-AP13)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF14">
-        <f>AG14/10*BV14+(AQ14-AQ13)</f>
+        <f t="shared" si="16"/>
         <v>23</v>
       </c>
       <c r="CG14">
-        <f>AH14/10*BW14+(AR14-AR13)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH14" s="1">
-        <f>BX14/AI14</f>
+        <f t="shared" si="0"/>
         <v>0.21818181818181817</v>
       </c>
       <c r="CI14" s="1">
-        <f>BY14/AJ14</f>
+        <f t="shared" si="1"/>
         <v>0.24324324324324326</v>
       </c>
       <c r="CJ14" s="1">
-        <f>BZ14/AK14</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK14" s="1">
-        <f>CA14/AL14</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL14" s="1">
-        <f>CB14/AM14</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM14" s="1">
-        <f>CC14/AN14</f>
+        <f t="shared" si="5"/>
         <v>0.21951219512195122</v>
       </c>
       <c r="CN14" s="1">
-        <f>CD14/AO14</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO14" s="1">
-        <f>CE14/AP14</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP14" s="1">
-        <f>CF14/AQ14</f>
+        <f t="shared" si="8"/>
         <v>0.28048780487804881</v>
       </c>
       <c r="CQ14" s="1">
-        <f>CG14/AR14</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -83263,81 +83253,81 @@
         <v>0</v>
       </c>
       <c r="BX15">
-        <f>Y15/10*BN15+(AI15-AI14)</f>
+        <f t="shared" si="14"/>
         <v>-10</v>
       </c>
       <c r="BY15">
-        <f>Z15/10*BO15+(AJ15-AJ14)</f>
+        <f t="shared" si="18"/>
         <v>-14</v>
       </c>
       <c r="BZ15">
         <v>0</v>
       </c>
       <c r="CA15">
-        <f>AB15/10*BQ15+(AL15-AL14)</f>
+        <f t="shared" ref="CA15:CA20" si="19">AB15/10*BQ15+(AL15-AL14)</f>
         <v>0</v>
       </c>
       <c r="CB15">
         <v>0</v>
       </c>
       <c r="CC15">
-        <f>AD15/10*BS15+(AN15-AN14)</f>
+        <f t="shared" si="15"/>
         <v>-16</v>
       </c>
       <c r="CD15">
-        <f>AE15/10*BT15+(AO15-AO14)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE15">
-        <f>AF15/10*BU15+(AP15-AP14)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF15">
-        <f>AG15/10*BV15+(AQ15-AQ14)</f>
+        <f t="shared" si="16"/>
         <v>-8</v>
       </c>
       <c r="CG15">
-        <f>AH15/10*BW15+(AR15-AR14)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH15" s="1">
-        <f>BX15/AI15</f>
+        <f t="shared" si="0"/>
         <v>-0.1</v>
       </c>
       <c r="CI15" s="1">
-        <f>BY15/AJ15</f>
+        <f t="shared" si="1"/>
         <v>-0.23333333333333334</v>
       </c>
       <c r="CJ15" s="1">
-        <f>BZ15/AK15</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK15" s="1">
-        <f>CA15/AL15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL15" s="1">
-        <f>CB15/AM15</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM15" s="1">
-        <f>CC15/AN15</f>
+        <f t="shared" si="5"/>
         <v>-0.24242424242424243</v>
       </c>
       <c r="CN15" s="1">
-        <f>CD15/AO15</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO15" s="1">
-        <f>CE15/AP15</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP15" s="1">
-        <f>CF15/AQ15</f>
+        <f t="shared" si="8"/>
         <v>-0.10810810810810811</v>
       </c>
       <c r="CQ15" s="1">
-        <f>CG15/AR15</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -83568,83 +83558,83 @@
         <v>1</v>
       </c>
       <c r="BX16">
-        <f>Y16/10*BN16+(AI16-AI15)</f>
+        <f t="shared" si="14"/>
         <v>27</v>
       </c>
       <c r="BY16">
-        <f>Z16/10*BO16+(AJ16-AJ15)</f>
+        <f t="shared" si="18"/>
         <v>-5</v>
       </c>
       <c r="BZ16">
-        <f>AA16/10*BP16+(AK16-AK15)</f>
+        <f t="shared" ref="BZ16:BZ26" si="20">AA16/10*BP16+(AK16-AK15)</f>
         <v>10</v>
       </c>
       <c r="CA16">
-        <f>AB16/10*BQ16+(AL16-AL15)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="CB16">
-        <f>AC16/10*BR16+(AM16-AM15)</f>
+        <f t="shared" ref="CB16:CB26" si="21">AC16/10*BR16+(AM16-AM15)</f>
         <v>14</v>
       </c>
       <c r="CC16">
-        <f>AD16/10*BS16+(AN16-AN15)</f>
+        <f t="shared" si="15"/>
         <v>-6</v>
       </c>
       <c r="CD16">
-        <f>AE16/10*BT16+(AO16-AO15)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE16">
-        <f>AF16/10*BU16+(AP16-AP15)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF16">
-        <f>AG16/10*BV16+(AQ16-AQ15)</f>
+        <f t="shared" si="16"/>
         <v>25</v>
       </c>
       <c r="CG16">
-        <f>AH16/10*BW16+(AR16-AR15)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH16" s="1">
-        <f>BX16/AI16</f>
+        <f t="shared" si="0"/>
         <v>0.24545454545454545</v>
       </c>
       <c r="CI16" s="1">
-        <f>BY16/AJ16</f>
+        <f t="shared" si="1"/>
         <v>-9.0909090909090912E-2</v>
       </c>
       <c r="CJ16" s="1">
-        <f>BZ16/AK16</f>
+        <f t="shared" si="2"/>
         <v>0.10989010989010989</v>
       </c>
       <c r="CK16" s="1">
-        <f>CA16/AL16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL16" s="1">
-        <f>CB16/AM16</f>
+        <f t="shared" si="4"/>
         <v>0.1891891891891892</v>
       </c>
       <c r="CM16" s="1">
-        <f>CC16/AN16</f>
+        <f t="shared" si="5"/>
         <v>-0.1</v>
       </c>
       <c r="CN16" s="1">
-        <f>CD16/AO16</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO16" s="1">
-        <f>CE16/AP16</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP16" s="1">
-        <f>CF16/AQ16</f>
+        <f t="shared" si="8"/>
         <v>0.3048780487804878</v>
       </c>
       <c r="CQ16" s="1">
-        <f>CG16/AR16</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -83875,83 +83865,83 @@
         <v>1</v>
       </c>
       <c r="BX17">
-        <f>Y17/10*BN17+(AI17-AI16)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BY17">
-        <f>Z17/10*BO17+(AJ17-AJ16)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BZ17">
-        <f>AA17/10*BP17+(AK17-AK16)</f>
+        <f t="shared" si="20"/>
         <v>22</v>
       </c>
       <c r="CA17">
-        <f>AB17/10*BQ17+(AL17-AL16)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="CB17">
-        <f>AC17/10*BR17+(AM17-AM16)</f>
+        <f t="shared" si="21"/>
         <v>18</v>
       </c>
       <c r="CC17">
-        <f>AD17/10*BS17+(AN17-AN16)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="CD17">
-        <f>AE17/10*BT17+(AO17-AO16)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="CE17">
-        <f>AF17/10*BU17+(AP17-AP16)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="CF17">
-        <f>AG17/10*BV17+(AQ17-AQ16)</f>
+        <f t="shared" si="16"/>
         <v>31</v>
       </c>
       <c r="CG17">
-        <f>AH17/10*BW17+(AR17-AR16)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH17" s="1">
-        <f>BX17/AI17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="CI17" s="1">
-        <f>BY17/AJ17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ17" s="1">
-        <f>BZ17/AK17</f>
+        <f t="shared" si="2"/>
         <v>0.22</v>
       </c>
       <c r="CK17" s="1">
-        <f>CA17/AL17</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL17" s="1">
-        <f>CB17/AM17</f>
+        <f t="shared" si="4"/>
         <v>0.21951219512195122</v>
       </c>
       <c r="CM17" s="1">
-        <f>CC17/AN17</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CN17" s="1">
-        <f>CD17/AO17</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO17" s="1">
-        <f>CE17/AP17</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP17" s="1">
-        <f>CF17/AQ17</f>
+        <f t="shared" si="8"/>
         <v>0.34065934065934067</v>
       </c>
       <c r="CQ17" s="1">
-        <f>CG17/AR17</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -84182,82 +84172,82 @@
         <v>0</v>
       </c>
       <c r="BX18">
-        <f>Y18/10*BN18+(AI18-AI17)</f>
+        <f t="shared" si="14"/>
         <v>-10</v>
       </c>
       <c r="BY18">
-        <f>Z18/10*BO18+(AJ18-AJ17)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BZ18">
-        <f>AA18/10*BP18+(AK18-AK17)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="CA18">
-        <f>AB18/10*BQ18+(AL18-AL17)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="CB18">
-        <f>AC18/10*BR18+(AM18-AM17)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="CC18">
-        <f>AD18/10*BS18+(AN18-AN17)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="CD18">
         <v>0</v>
       </c>
       <c r="CE18">
-        <f>AF18/10*BU18+(AP18-AP17)</f>
+        <f t="shared" ref="CE18:CE23" si="22">AF18/10*BU18+(AP18-AP17)</f>
         <v>0</v>
       </c>
       <c r="CF18">
-        <f>AG18/10*BV18+(AQ18-AQ17)</f>
+        <f t="shared" si="16"/>
         <v>-17</v>
       </c>
       <c r="CG18">
-        <f>AH18/10*BW18+(AR18-AR17)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH18" s="1">
-        <f>BX18/AI18</f>
+        <f t="shared" si="0"/>
         <v>-0.1</v>
       </c>
       <c r="CI18" s="1">
-        <f>BY18/AJ18</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ18" s="1">
-        <f>BZ18/AK18</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK18" s="1">
-        <f>CA18/AL18</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL18" s="1">
-        <f>CB18/AM18</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM18" s="1">
-        <f>CC18/AN18</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CN18" s="1">
-        <f>CD18/AO18</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO18" s="1">
-        <f>CE18/AP18</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP18" s="1">
-        <f>CF18/AQ18</f>
+        <f t="shared" si="8"/>
         <v>-0.22972972972972974</v>
       </c>
       <c r="CQ18" s="1">
-        <f>CG18/AR18</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -84488,83 +84478,83 @@
         <v>1</v>
       </c>
       <c r="BX19">
-        <f>Y19/10*BN19+(AI19-AI18)</f>
+        <f t="shared" si="14"/>
         <v>22</v>
       </c>
       <c r="BY19">
-        <f>Z19/10*BO19+(AJ19-AJ18)</f>
+        <f t="shared" si="18"/>
         <v>-5</v>
       </c>
       <c r="BZ19">
-        <f>AA19/10*BP19+(AK19-AK18)</f>
+        <f t="shared" si="20"/>
         <v>27</v>
       </c>
       <c r="CA19">
-        <f>AB19/10*BQ19+(AL19-AL18)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="CB19">
-        <f>AC19/10*BR19+(AM19-AM18)</f>
+        <f t="shared" si="21"/>
         <v>31</v>
       </c>
       <c r="CC19">
-        <f>AD19/10*BS19+(AN19-AN18)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="CD19">
-        <f>AE19/10*BT19+(AO19-AO18)</f>
+        <f t="shared" ref="CD19:CD26" si="23">AE19/10*BT19+(AO19-AO18)</f>
         <v>15</v>
       </c>
       <c r="CE19">
-        <f>AF19/10*BU19+(AP19-AP18)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="CF19">
-        <f>AG19/10*BV19+(AQ19-AQ18)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="CG19">
-        <f>AH19/10*BW19+(AR19-AR18)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH19" s="1">
-        <f>BX19/AI19</f>
+        <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
       <c r="CI19" s="1">
-        <f>BY19/AJ19</f>
+        <f t="shared" si="1"/>
         <v>-0.1</v>
       </c>
       <c r="CJ19" s="1">
-        <f>BZ19/AK19</f>
+        <f t="shared" si="2"/>
         <v>0.24545454545454545</v>
       </c>
       <c r="CK19" s="1">
-        <f>CA19/AL19</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL19" s="1">
-        <f>CB19/AM19</f>
+        <f t="shared" si="4"/>
         <v>0.34065934065934067</v>
       </c>
       <c r="CM19" s="1">
-        <f>CC19/AN19</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CN19" s="1">
-        <f>CD19/AO19</f>
+        <f t="shared" si="6"/>
         <v>0.15</v>
       </c>
       <c r="CO19" s="1">
-        <f>CE19/AP19</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP19" s="1">
-        <f>CF19/AQ19</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="CQ19" s="1">
-        <f>CG19/AR19</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -84795,83 +84785,83 @@
         <v>1</v>
       </c>
       <c r="BX20">
-        <f>Y20/10*BN20+(AI20-AI19)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BY20">
-        <f>Z20/10*BO20+(AJ20-AJ19)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BZ20">
-        <f>AA20/10*BP20+(AK20-AK19)</f>
+        <f t="shared" si="20"/>
         <v>32</v>
       </c>
       <c r="CA20">
-        <f>AB20/10*BQ20+(AL20-AL19)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="CB20">
-        <f>AC20/10*BR20+(AM20-AM19)</f>
+        <f t="shared" si="21"/>
         <v>33</v>
       </c>
       <c r="CC20">
-        <f>AD20/10*BS20+(AN20-AN19)</f>
+        <f t="shared" si="15"/>
         <v>31</v>
       </c>
       <c r="CD20">
-        <f>AE20/10*BT20+(AO20-AO19)</f>
+        <f t="shared" si="23"/>
         <v>20</v>
       </c>
       <c r="CE20">
-        <f>AF20/10*BU20+(AP20-AP19)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="CF20">
-        <f>AG20/10*BV20+(AQ20-AQ19)</f>
+        <f t="shared" si="16"/>
         <v>40</v>
       </c>
       <c r="CG20">
-        <f>AH20/10*BW20+(AR20-AR19)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="CH20" s="1">
-        <f>BX20/AI20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="CI20" s="1">
-        <f>BY20/AJ20</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ20" s="1">
-        <f>BZ20/AK20</f>
+        <f t="shared" si="2"/>
         <v>0.26446280991735538</v>
       </c>
       <c r="CK20" s="1">
-        <f>CA20/AL20</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL20" s="1">
-        <f>CB20/AM20</f>
+        <f t="shared" si="4"/>
         <v>0.33</v>
       </c>
       <c r="CM20" s="1">
-        <f>CC20/AN20</f>
+        <f t="shared" si="5"/>
         <v>0.46969696969696972</v>
       </c>
       <c r="CN20" s="1">
-        <f>CD20/AO20</f>
+        <f t="shared" si="6"/>
         <v>0.18181818181818182</v>
       </c>
       <c r="CO20" s="1">
-        <f>CE20/AP20</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP20" s="1">
-        <f>CF20/AQ20</f>
+        <f t="shared" si="8"/>
         <v>0.48780487804878048</v>
       </c>
       <c r="CQ20" s="1">
-        <f>CG20/AR20</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -85102,81 +85092,81 @@
         <v>0</v>
       </c>
       <c r="BX21">
-        <f>Y21/10*BN21+(AI21-AI20)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BY21">
-        <f>Z21/10*BO21+(AJ21-AJ20)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BZ21">
-        <f>AA21/10*BP21+(AK21-AK20)</f>
+        <f t="shared" si="20"/>
         <v>-21</v>
       </c>
       <c r="CA21">
         <v>0</v>
       </c>
       <c r="CB21">
-        <f>AC21/10*BR21+(AM21-AM20)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="CC21">
-        <f>AD21/10*BS21+(AN21-AN20)</f>
+        <f t="shared" si="15"/>
         <v>-11</v>
       </c>
       <c r="CD21">
-        <f>AE21/10*BT21+(AO21-AO20)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="CE21">
-        <f>AF21/10*BU21+(AP21-AP20)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="CF21">
-        <f>AG21/10*BV21+(AQ21-AQ20)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="CG21">
         <v>0</v>
       </c>
       <c r="CH21" s="1">
-        <f>BX21/AI21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="CI21" s="1">
-        <f>BY21/AJ21</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ21" s="1">
-        <f>BZ21/AK21</f>
+        <f t="shared" si="2"/>
         <v>-0.21</v>
       </c>
       <c r="CK21" s="1">
-        <f>CA21/AL21</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL21" s="1">
-        <f>CB21/AM21</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM21" s="1">
-        <f>CC21/AN21</f>
+        <f t="shared" si="5"/>
         <v>-0.2</v>
       </c>
       <c r="CN21" s="1">
-        <f>CD21/AO21</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO21" s="1">
-        <f>CE21/AP21</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP21" s="1">
-        <f>CF21/AQ21</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="CQ21" s="1">
-        <f>CG21/AR21</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -85407,15 +85397,15 @@
         <v>1</v>
       </c>
       <c r="BX22">
-        <f>Y22/10*BN22+(AI22-AI21)</f>
+        <f t="shared" si="14"/>
         <v>10</v>
       </c>
       <c r="BY22">
-        <f>Z22/10*BO22+(AJ22-AJ21)</f>
+        <f t="shared" si="18"/>
         <v>16</v>
       </c>
       <c r="BZ22">
-        <f>AA22/10*BP22+(AK22-AK21)</f>
+        <f t="shared" si="20"/>
         <v>25</v>
       </c>
       <c r="CA22">
@@ -85423,23 +85413,23 @@
         <v>22</v>
       </c>
       <c r="CB22">
-        <f>AC22/10*BR22+(AM22-AM21)</f>
+        <f t="shared" si="21"/>
         <v>37</v>
       </c>
       <c r="CC22">
-        <f>AD22/10*BS22+(AN22-AN21)</f>
+        <f t="shared" si="15"/>
         <v>37</v>
       </c>
       <c r="CD22">
-        <f>AE22/10*BT22+(AO22-AO21)</f>
+        <f t="shared" si="23"/>
         <v>38</v>
       </c>
       <c r="CE22">
-        <f>AF22/10*BU22+(AP22-AP21)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="CF22">
-        <f>AG22/10*BV22+(AQ22-AQ21)</f>
+        <f t="shared" si="16"/>
         <v>47</v>
       </c>
       <c r="CG22">
@@ -85447,43 +85437,43 @@
         <v>23</v>
       </c>
       <c r="CH22" s="1">
-        <f>BX22/AI22</f>
+        <f t="shared" si="0"/>
         <v>9.0909090909090912E-2</v>
       </c>
       <c r="CI22" s="1">
-        <f>BY22/AJ22</f>
+        <f t="shared" si="1"/>
         <v>0.29090909090909089</v>
       </c>
       <c r="CJ22" s="1">
-        <f>BZ22/AK22</f>
+        <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
       <c r="CK22" s="1">
-        <f>CA22/AL22</f>
+        <f t="shared" si="3"/>
         <v>0.22</v>
       </c>
       <c r="CL22" s="1">
-        <f>CB22/AM22</f>
+        <f t="shared" si="4"/>
         <v>0.33636363636363636</v>
       </c>
       <c r="CM22" s="1">
-        <f>CC22/AN22</f>
+        <f t="shared" si="5"/>
         <v>0.6166666666666667</v>
       </c>
       <c r="CN22" s="1">
-        <f>CD22/AO22</f>
+        <f t="shared" si="6"/>
         <v>0.31404958677685951</v>
       </c>
       <c r="CO22" s="1">
-        <f>CE22/AP22</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP22" s="1">
-        <f>CF22/AQ22</f>
+        <f t="shared" si="8"/>
         <v>0.51648351648351654</v>
       </c>
       <c r="CQ22" s="1">
-        <f>CG22/AR22</f>
+        <f t="shared" si="9"/>
         <v>0.25274725274725274</v>
       </c>
     </row>
@@ -85714,15 +85704,15 @@
         <v>1</v>
       </c>
       <c r="BX23">
-        <f>Y23/10*BN23+(AI23-AI22)</f>
+        <f t="shared" si="14"/>
         <v>46</v>
       </c>
       <c r="BY23">
-        <f>Z23/10*BO23+(AJ23-AJ22)</f>
+        <f t="shared" si="18"/>
         <v>11</v>
       </c>
       <c r="BZ23">
-        <f>AA23/10*BP23+(AK23-AK22)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="CA23">
@@ -85730,23 +85720,23 @@
         <v>33</v>
       </c>
       <c r="CB23">
-        <f>AC23/10*BR23+(AM23-AM22)</f>
+        <f t="shared" si="21"/>
         <v>39</v>
       </c>
       <c r="CC23">
-        <f>AD23/10*BS23+(AN23-AN22)</f>
+        <f t="shared" si="15"/>
         <v>39</v>
       </c>
       <c r="CD23">
-        <f>AE23/10*BT23+(AO23-AO22)</f>
+        <f t="shared" si="23"/>
         <v>27</v>
       </c>
       <c r="CE23">
-        <f>AF23/10*BU23+(AP23-AP22)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="CF23">
-        <f>AG23/10*BV23+(AQ23-AQ22)</f>
+        <f t="shared" si="16"/>
         <v>49</v>
       </c>
       <c r="CG23">
@@ -85754,43 +85744,43 @@
         <v>26</v>
       </c>
       <c r="CH23" s="1">
-        <f>BX23/AI23</f>
+        <f t="shared" si="0"/>
         <v>0.38016528925619836</v>
       </c>
       <c r="CI23" s="1">
-        <f>BY23/AJ23</f>
+        <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
       <c r="CJ23" s="1">
-        <f>BZ23/AK23</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK23" s="1">
-        <f>CA23/AL23</f>
+        <f t="shared" si="3"/>
         <v>0.3</v>
       </c>
       <c r="CL23" s="1">
-        <f>CB23/AM23</f>
+        <f t="shared" si="4"/>
         <v>0.32231404958677684</v>
       </c>
       <c r="CM23" s="1">
-        <f>CC23/AN23</f>
+        <f t="shared" si="5"/>
         <v>0.59090909090909094</v>
       </c>
       <c r="CN23" s="1">
-        <f>CD23/AO23</f>
+        <f t="shared" si="6"/>
         <v>0.2231404958677686</v>
       </c>
       <c r="CO23" s="1">
-        <f>CE23/AP23</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP23" s="1">
-        <f>CF23/AQ23</f>
+        <f t="shared" si="8"/>
         <v>0.49</v>
       </c>
       <c r="CQ23" s="1">
-        <f>CG23/AR23</f>
+        <f t="shared" si="9"/>
         <v>0.26</v>
       </c>
     </row>
@@ -86021,15 +86011,15 @@
         <v>0</v>
       </c>
       <c r="BX24">
-        <f>Y24/10*BN24+(AI24-AI23)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="BY24">
-        <f>Z24/10*BO24+(AJ24-AJ23)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="BZ24">
-        <f>AA24/10*BP24+(AK24-AK23)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="CA24">
@@ -86037,22 +86027,22 @@
         <v>0</v>
       </c>
       <c r="CB24">
-        <f>AC24/10*BR24+(AM24-AM23)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="CC24">
-        <f>AD24/10*BS24+(AN24-AN23)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="CD24">
-        <f>AE24/10*BT24+(AO24-AO23)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="CE24">
         <v>0</v>
       </c>
       <c r="CF24">
-        <f>AG24/10*BV24+(AQ24-AQ23)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="CG24">
@@ -86060,43 +86050,43 @@
         <v>0</v>
       </c>
       <c r="CH24" s="1">
-        <f>BX24/AI24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="CI24" s="1">
-        <f>BY24/AJ24</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="CJ24" s="1">
-        <f>BZ24/AK24</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="CK24" s="1">
-        <f>CA24/AL24</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="CL24" s="1">
-        <f>CB24/AM24</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="CM24" s="1">
-        <f>CC24/AN24</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="CN24" s="1">
-        <f>CD24/AO24</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="CO24" s="1">
-        <f>CE24/AP24</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="CP24" s="1">
-        <f>CF24/AQ24</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="CQ24" s="1">
-        <f>CG24/AR24</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -86327,15 +86317,15 @@
         <v>1</v>
       </c>
       <c r="BX25">
-        <f>Y25/10*BN25+(AI25-AI24)</f>
+        <f t="shared" si="14"/>
         <v>48</v>
       </c>
       <c r="BY25">
-        <f>Z25/10*BO25+(AJ25-AJ24)</f>
+        <f t="shared" si="18"/>
         <v>24</v>
       </c>
       <c r="BZ25">
-        <f>AA25/10*BP25+(AK25-AK24)</f>
+        <f t="shared" si="20"/>
         <v>43</v>
       </c>
       <c r="CA25">
@@ -86343,15 +86333,15 @@
         <v>35</v>
       </c>
       <c r="CB25">
-        <f>AC25/10*BR25+(AM25-AM24)</f>
+        <f t="shared" si="21"/>
         <v>41</v>
       </c>
       <c r="CC25">
-        <f>AD25/10*BS25+(AN25-AN24)</f>
+        <f t="shared" si="15"/>
         <v>44</v>
       </c>
       <c r="CD25">
-        <f>AE25/10*BT25+(AO25-AO24)</f>
+        <f t="shared" si="23"/>
         <v>27</v>
       </c>
       <c r="CE25">
@@ -86359,7 +86349,7 @@
         <v>18</v>
       </c>
       <c r="CF25">
-        <f>AG25/10*BV25+(AQ25-AQ24)</f>
+        <f t="shared" si="16"/>
         <v>40</v>
       </c>
       <c r="CG25">
@@ -86367,43 +86357,43 @@
         <v>17</v>
       </c>
       <c r="CH25" s="1">
-        <f>BX25/AI25</f>
+        <f t="shared" si="0"/>
         <v>0.36090225563909772</v>
       </c>
       <c r="CI25" s="1">
-        <f>BY25/AJ25</f>
+        <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
       <c r="CJ25" s="1">
-        <f>BZ25/AK25</f>
+        <f t="shared" si="2"/>
         <v>0.39090909090909093</v>
       </c>
       <c r="CK25" s="1">
-        <f>CA25/AL25</f>
+        <f t="shared" si="3"/>
         <v>0.28925619834710742</v>
       </c>
       <c r="CL25" s="1">
-        <f>CB25/AM25</f>
+        <f t="shared" si="4"/>
         <v>0.30827067669172931</v>
       </c>
       <c r="CM25" s="1">
-        <f>CC25/AN25</f>
+        <f t="shared" si="5"/>
         <v>0.59459459459459463</v>
       </c>
       <c r="CN25" s="1">
-        <f>CD25/AO25</f>
+        <f t="shared" si="6"/>
         <v>0.2231404958677686</v>
       </c>
       <c r="CO25" s="1">
-        <f>CE25/AP25</f>
+        <f t="shared" si="7"/>
         <v>0.19780219780219779</v>
       </c>
       <c r="CP25" s="1">
-        <f>CF25/AQ25</f>
+        <f t="shared" si="8"/>
         <v>0.4</v>
       </c>
       <c r="CQ25" s="1">
-        <f>CG25/AR25</f>
+        <f t="shared" si="9"/>
         <v>0.17</v>
       </c>
     </row>
@@ -86634,15 +86624,15 @@
         <v>1</v>
       </c>
       <c r="BX26">
-        <f>Y26/10*BN26+(AI26-AI25)</f>
+        <f t="shared" si="14"/>
         <v>52</v>
       </c>
       <c r="BY26">
-        <f>Z26/10*BO26+(AJ26-AJ25)</f>
+        <f t="shared" si="18"/>
         <v>19</v>
       </c>
       <c r="BZ26">
-        <f>AA26/10*BP26+(AK26-AK25)</f>
+        <f t="shared" si="20"/>
         <v>49</v>
       </c>
       <c r="CA26">
@@ -86650,15 +86640,15 @@
         <v>40</v>
       </c>
       <c r="CB26">
-        <f>AC26/10*BR26+(AM26-AM25)</f>
+        <f t="shared" si="21"/>
         <v>46</v>
       </c>
       <c r="CC26">
-        <f>AD26/10*BS26+(AN26-AN25)</f>
+        <f t="shared" si="15"/>
         <v>45</v>
       </c>
       <c r="CD26">
-        <f>AE26/10*BT26+(AO26-AO25)</f>
+        <f t="shared" si="23"/>
         <v>42</v>
       </c>
       <c r="CE26">
@@ -86666,7 +86656,7 @@
         <v>23</v>
       </c>
       <c r="CF26">
-        <f>AG26/10*BV26+(AQ26-AQ25)</f>
+        <f t="shared" si="16"/>
         <v>54</v>
       </c>
       <c r="CG26">
@@ -86674,44 +86664,50 @@
         <v>31</v>
       </c>
       <c r="CH26" s="1">
-        <f>BX26/AI26</f>
+        <f t="shared" si="0"/>
         <v>0.35616438356164382</v>
       </c>
       <c r="CI26" s="1">
-        <f>BY26/AJ26</f>
+        <f t="shared" si="1"/>
         <v>0.31666666666666665</v>
       </c>
       <c r="CJ26" s="1">
-        <f>BZ26/AK26</f>
+        <f t="shared" si="2"/>
         <v>0.4049586776859504</v>
       </c>
       <c r="CK26" s="1">
-        <f>CA26/AL26</f>
+        <f t="shared" si="3"/>
         <v>0.3007518796992481</v>
       </c>
       <c r="CL26" s="1">
-        <f>CB26/AM26</f>
+        <f t="shared" si="4"/>
         <v>0.31506849315068491</v>
       </c>
       <c r="CM26" s="1">
-        <f>CC26/AN26</f>
+        <f t="shared" si="5"/>
         <v>0.54878048780487809</v>
       </c>
       <c r="CN26" s="1">
-        <f>CD26/AO26</f>
+        <f t="shared" si="6"/>
         <v>0.31578947368421051</v>
       </c>
       <c r="CO26" s="1">
-        <f>CE26/AP26</f>
+        <f t="shared" si="7"/>
         <v>0.23</v>
       </c>
       <c r="CP26" s="1">
-        <f>CF26/AQ26</f>
+        <f t="shared" si="8"/>
         <v>0.49090909090909091</v>
       </c>
       <c r="CQ26" s="1">
-        <f>CG26/AR26</f>
+        <f t="shared" si="9"/>
         <v>0.2818181818181818</v>
+      </c>
+    </row>
+    <row r="27" spans="1:95" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <f>SUM(J26:N26)</f>
+        <v>19759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>